<commit_message>
Worked on spice models.
</commit_message>
<xml_diff>
--- a/driver_cplex_rp2040/production/ver0p1_rev1/CPL_JLCPCB_cplex_rp2040_v0p1_r1.xlsx
+++ b/driver_cplex_rp2040/production/ver0p1_rev1/CPL_JLCPCB_cplex_rp2040_v0p1_r1.xlsx
@@ -1487,7 +1487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1516,6 +1516,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1573,7 +1579,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1587,6 +1593,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1609,8 +1619,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2081,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="1" t="n">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,8 +2107,8 @@
       <c r="D28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="1" t="n">
-        <v>180</v>
+      <c r="E28" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2114,8 +2124,8 @@
       <c r="D29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="1" t="n">
-        <v>180</v>
+      <c r="E29" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,8 +2141,8 @@
       <c r="D30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="1" t="n">
-        <v>180</v>
+      <c r="E30" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,8 +2158,8 @@
       <c r="D31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="1" t="n">
-        <v>180</v>
+      <c r="E31" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,8 +2175,8 @@
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="1" t="n">
-        <v>180</v>
+      <c r="E32" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,8 +2192,8 @@
       <c r="D33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="1" t="n">
-        <v>180</v>
+      <c r="E33" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,8 +2209,8 @@
       <c r="D34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="1" t="n">
-        <v>180</v>
+      <c r="E34" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,8 +2226,8 @@
       <c r="D35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="1" t="n">
-        <v>180</v>
+      <c r="E35" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,8 +2243,8 @@
       <c r="D36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="1" t="n">
-        <v>180</v>
+      <c r="E36" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,8 +2260,8 @@
       <c r="D37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="1" t="n">
-        <v>180</v>
+      <c r="E37" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,8 +2277,8 @@
       <c r="D38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="1" t="n">
-        <v>180</v>
+      <c r="E38" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,8 +2294,8 @@
       <c r="D39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="1" t="n">
-        <v>180</v>
+      <c r="E39" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,8 +2311,8 @@
       <c r="D40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="1" t="n">
-        <v>180</v>
+      <c r="E40" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,8 +2328,8 @@
       <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="1" t="n">
-        <v>180</v>
+      <c r="E41" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,8 +2345,8 @@
       <c r="D42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="1" t="n">
-        <v>180</v>
+      <c r="E42" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,8 +2362,8 @@
       <c r="D43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="1" t="n">
-        <v>180</v>
+      <c r="E43" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,8 +2379,8 @@
       <c r="D44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="1" t="n">
-        <v>180</v>
+      <c r="E44" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,8 +2396,8 @@
       <c r="D45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="1" t="n">
-        <v>180</v>
+      <c r="E45" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,8 +2413,8 @@
       <c r="D46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="1" t="n">
-        <v>180</v>
+      <c r="E46" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,8 +2430,8 @@
       <c r="D47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="1" t="n">
-        <v>180</v>
+      <c r="E47" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,8 +2447,8 @@
       <c r="D48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="1" t="n">
-        <v>180</v>
+      <c r="E48" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,8 +2464,8 @@
       <c r="D49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="1" t="n">
-        <v>180</v>
+      <c r="E49" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,8 +2481,8 @@
       <c r="D50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="1" t="n">
-        <v>180</v>
+      <c r="E50" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,8 +2498,8 @@
       <c r="D51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="1" t="n">
-        <v>180</v>
+      <c r="E51" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,8 +2515,8 @@
       <c r="D52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="1" t="n">
-        <v>180</v>
+      <c r="E52" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,8 +2532,8 @@
       <c r="D53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="1" t="n">
-        <v>180</v>
+      <c r="E53" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,8 +2549,8 @@
       <c r="D54" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="1" t="n">
-        <v>180</v>
+      <c r="E54" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,8 +2566,8 @@
       <c r="D55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="1" t="n">
-        <v>180</v>
+      <c r="E55" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,8 +2583,8 @@
       <c r="D56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="1" t="n">
-        <v>180</v>
+      <c r="E56" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,8 +2600,8 @@
       <c r="D57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="1" t="n">
-        <v>180</v>
+      <c r="E57" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,8 +2617,8 @@
       <c r="D58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="1" t="n">
-        <v>180</v>
+      <c r="E58" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,8 +2634,8 @@
       <c r="D59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="1" t="n">
-        <v>180</v>
+      <c r="E59" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2641,8 +2651,8 @@
       <c r="D60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="1" t="n">
-        <v>180</v>
+      <c r="E60" s="4" t="n">
+        <v>-90</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5379,7 +5389,7 @@
         <v>6</v>
       </c>
       <c r="E221" s="1" t="n">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>